<commit_message>
2 bytes with duplicate and 4 bytes
</commit_message>
<xml_diff>
--- a/Moderate Control Signature for Each Two Bytes.xlsx
+++ b/Moderate Control Signature for Each Two Bytes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FYP\Tianyu Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF79042B-1573-4E68-BF08-E73D526F7D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630A1FDB-20A7-4AED-AF2D-B4F27D772C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15372" yWindow="2520" windowWidth="12108" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2412" yWindow="3888" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Byte 0&amp;1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
-  <si>
-    <t>Δ42 = Δ46 = 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Target Register</t>
   </si>
@@ -46,6 +43,27 @@
   </si>
   <si>
     <t>Remarks/Comments</t>
+  </si>
+  <si>
+    <t>Δ56 = 1 and (Δ42 != 1 and Δ62!=1 and Δ74 != 1 and Δ78 != 1) and (Δ42!= 1 and Δ74!= 1 and Δ78!= 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Δ58=1 and Δ44!= 1 and  Δ64 != 1 and Δ80 != 1 ) </t>
+  </si>
+  <si>
+    <t>Δ60=1 and (Δ50 !=1 and Δ66!= 1 and Δ78!= 1 and Δ82!= 1 and Δ98!=1)</t>
+  </si>
+  <si>
+    <t>Δ62=1 and (Δ52!=1 and Δ80!= 1 and Δ84!= 1 and Δ100!=1)</t>
+  </si>
+  <si>
+    <t>Δ50=1 and (Δ36!= 1 and Δ40!= 1 and Δ56 !=1 and Δ88!= 1 ) and (Δ84 != 1)</t>
+  </si>
+  <si>
+    <t>Δ52 = 1 and (Δ38 != 1 and Δ42 != 1 and Δ58!= 1 and Δ70 != 1 and Δ74 != 1) and (Δ86 != 1 and Δ92 != 1)</t>
+  </si>
+  <si>
+    <t>Δ54=1 and (Δ40 != 1 and/or? Δ44 != 1 and Δ60 !=1 and Δ92 != 1) and (Δ40 !=1 and Δ88 !=1)</t>
   </si>
 </sst>
 </file>
@@ -93,12 +111,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -381,28 +402,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="46.44140625" customWidth="1"/>
+    <col min="2" max="2" width="93.88671875" customWidth="1"/>
     <col min="3" max="3" width="44.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -410,7 +431,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -421,8 +442,11 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -436,6 +460,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -448,11 +475,71 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -478,13 +565,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>